<commit_message>
Fix report-checklist.xlsx: Remove valorization from column L for tests 159,162,164-168
Corrected validation error C012 reported by ministerial validator:
Column L should NOT be valorized for test cases 159, 162, 164, 165, 166, 167, 168.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRSA/0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HNRSA/0.1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TMP\Collaudo RSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B7910A-D4B0-45E7-959A-A44650C543F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5A9A11-0B4C-4689-9F35-1CBC37AEDA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="491">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -989,9 +989,6 @@
   </si>
   <si>
     <t>Campo/sezione non gestito/a in modo strutturato dall’applicativo</t>
-  </si>
-  <si>
-    <t>campo/sezione non gestito/a in modo strutturato dall'applicativo</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
@@ -2278,6 +2275,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2289,17 +2294,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -3749,7 +3746,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3791,14 +3788,14 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -3819,14 +3816,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="54"/>
+      <c r="D3" s="50"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -3847,12 +3844,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="56" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3874,12 +3871,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="56" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="50"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -3900,8 +3897,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="57"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -4241,10 +4238,10 @@
         <v>46011</v>
       </c>
       <c r="G15" s="37" t="s">
+        <v>456</v>
+      </c>
+      <c r="H15" s="37" t="s">
         <v>457</v>
-      </c>
-      <c r="H15" s="37" t="s">
-        <v>458</v>
       </c>
       <c r="I15" t="s">
         <v>63</v>
@@ -4561,10 +4558,10 @@
         <v>46011</v>
       </c>
       <c r="G23" s="37" t="s">
+        <v>458</v>
+      </c>
+      <c r="H23" s="37" t="s">
         <v>459</v>
-      </c>
-      <c r="H23" s="37" t="s">
-        <v>460</v>
       </c>
       <c r="I23" t="s">
         <v>63</v>
@@ -4889,7 +4886,7 @@
         <v>46011</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H31" s="37"/>
       <c r="I31" s="42"/>
@@ -8062,13 +8059,13 @@
         <v>46011</v>
       </c>
       <c r="G116" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="H116" s="37" t="s">
         <v>462</v>
       </c>
-      <c r="H116" s="37" t="s">
+      <c r="I116" s="42" t="s">
         <v>463</v>
-      </c>
-      <c r="I116" s="42" t="s">
-        <v>464</v>
       </c>
       <c r="J116" s="38" t="s">
         <v>64</v>
@@ -8123,13 +8120,13 @@
         <v>46011</v>
       </c>
       <c r="G117" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="H117" s="37" t="s">
         <v>465</v>
       </c>
-      <c r="H117" s="37" t="s">
+      <c r="I117" s="42" t="s">
         <v>466</v>
-      </c>
-      <c r="I117" s="42" t="s">
-        <v>467</v>
       </c>
       <c r="J117" s="38" t="s">
         <v>64</v>
@@ -8184,13 +8181,13 @@
         <v>46011</v>
       </c>
       <c r="G118" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="H118" s="37" t="s">
         <v>468</v>
       </c>
-      <c r="H118" s="37" t="s">
+      <c r="I118" s="42" t="s">
         <v>469</v>
-      </c>
-      <c r="I118" s="42" t="s">
-        <v>470</v>
       </c>
       <c r="J118" s="38" t="s">
         <v>64</v>
@@ -8245,13 +8242,13 @@
         <v>46011</v>
       </c>
       <c r="G119" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="H119" s="37" t="s">
         <v>471</v>
       </c>
-      <c r="H119" s="37" t="s">
+      <c r="I119" s="42" t="s">
         <v>472</v>
-      </c>
-      <c r="I119" s="42" t="s">
-        <v>473</v>
       </c>
       <c r="J119" s="38" t="s">
         <v>64</v>
@@ -8312,9 +8309,7 @@
       <c r="K120" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L120" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L120" s="38"/>
       <c r="M120" s="38"/>
       <c r="N120" s="38"/>
       <c r="P120" s="38"/>
@@ -8339,22 +8334,22 @@
         <v>61</v>
       </c>
       <c r="D121" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E121" s="43" t="s">
         <v>273</v>
-      </c>
-      <c r="E121" s="43" t="s">
-        <v>274</v>
       </c>
       <c r="F121" s="37">
         <v>46011</v>
       </c>
       <c r="G121" s="37" t="s">
+        <v>473</v>
+      </c>
+      <c r="H121" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="H121" s="37" t="s">
+      <c r="I121" s="42" t="s">
         <v>475</v>
-      </c>
-      <c r="I121" s="42" t="s">
-        <v>476</v>
       </c>
       <c r="J121" s="38" t="s">
         <v>64</v>
@@ -8368,7 +8363,7 @@
         <v>64</v>
       </c>
       <c r="O121" s="38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P121" s="38" t="s">
         <v>64</v>
@@ -8400,22 +8395,22 @@
         <v>61</v>
       </c>
       <c r="D122" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="E122" s="43" t="s">
         <v>276</v>
-      </c>
-      <c r="E122" s="43" t="s">
-        <v>277</v>
       </c>
       <c r="F122" s="37">
         <v>46011</v>
       </c>
       <c r="G122" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="H122" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="H122" s="37" t="s">
+      <c r="I122" s="42" t="s">
         <v>478</v>
-      </c>
-      <c r="I122" s="42" t="s">
-        <v>479</v>
       </c>
       <c r="J122" s="38" t="s">
         <v>64</v>
@@ -8429,7 +8424,7 @@
         <v>64</v>
       </c>
       <c r="O122" s="38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P122" s="38" t="s">
         <v>64</v>
@@ -8461,10 +8456,10 @@
         <v>61</v>
       </c>
       <c r="D123" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="E123" s="43" t="s">
         <v>279</v>
-      </c>
-      <c r="E123" s="43" t="s">
-        <v>280</v>
       </c>
       <c r="F123" s="37"/>
       <c r="G123" s="37"/>
@@ -8476,9 +8471,7 @@
       <c r="K123" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L123" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L123" s="38"/>
       <c r="M123" s="38"/>
       <c r="N123" s="38"/>
       <c r="O123" s="38"/>
@@ -8504,22 +8497,22 @@
         <v>61</v>
       </c>
       <c r="D124" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="E124" s="43" t="s">
         <v>281</v>
-      </c>
-      <c r="E124" s="43" t="s">
-        <v>282</v>
       </c>
       <c r="F124" s="37">
         <v>46011</v>
       </c>
       <c r="G124" s="37" t="s">
+        <v>479</v>
+      </c>
+      <c r="H124" s="37" t="s">
+        <v>481</v>
+      </c>
+      <c r="I124" s="42" t="s">
         <v>480</v>
-      </c>
-      <c r="H124" s="37" t="s">
-        <v>482</v>
-      </c>
-      <c r="I124" s="42" t="s">
-        <v>481</v>
       </c>
       <c r="J124" s="38" t="s">
         <v>64</v>
@@ -8533,7 +8526,7 @@
         <v>64</v>
       </c>
       <c r="O124" s="38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P124" s="38" t="s">
         <v>64</v>
@@ -8565,10 +8558,10 @@
         <v>61</v>
       </c>
       <c r="D125" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="E125" s="43" t="s">
         <v>283</v>
-      </c>
-      <c r="E125" s="43" t="s">
-        <v>284</v>
       </c>
       <c r="F125" s="37"/>
       <c r="G125" s="37"/>
@@ -8580,9 +8573,7 @@
       <c r="K125" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L125" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L125" s="38"/>
       <c r="M125" s="38"/>
       <c r="N125" s="38"/>
       <c r="O125" s="38"/>
@@ -8608,10 +8599,10 @@
         <v>61</v>
       </c>
       <c r="D126" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="E126" s="43" t="s">
         <v>285</v>
-      </c>
-      <c r="E126" s="43" t="s">
-        <v>286</v>
       </c>
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
@@ -8623,9 +8614,7 @@
       <c r="K126" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L126" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L126" s="38"/>
       <c r="M126" s="38"/>
       <c r="N126" s="38"/>
       <c r="O126" s="38"/>
@@ -8651,10 +8640,10 @@
         <v>61</v>
       </c>
       <c r="D127" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="E127" s="43" t="s">
         <v>287</v>
-      </c>
-      <c r="E127" s="43" t="s">
-        <v>288</v>
       </c>
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
@@ -8666,9 +8655,7 @@
       <c r="K127" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L127" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L127" s="38"/>
       <c r="M127" s="38"/>
       <c r="N127" s="38"/>
       <c r="O127" s="38"/>
@@ -8694,10 +8681,10 @@
         <v>61</v>
       </c>
       <c r="D128" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="E128" s="43" t="s">
         <v>289</v>
-      </c>
-      <c r="E128" s="43" t="s">
-        <v>290</v>
       </c>
       <c r="F128" s="37"/>
       <c r="G128" s="37"/>
@@ -8709,9 +8696,7 @@
       <c r="K128" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L128" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L128" s="38"/>
       <c r="M128" s="38"/>
       <c r="N128" s="38"/>
       <c r="O128" s="38"/>
@@ -8737,10 +8722,10 @@
         <v>61</v>
       </c>
       <c r="D129" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="E129" s="43" t="s">
         <v>291</v>
-      </c>
-      <c r="E129" s="43" t="s">
-        <v>292</v>
       </c>
       <c r="F129" s="37"/>
       <c r="G129" s="37"/>
@@ -8752,9 +8737,7 @@
       <c r="K129" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="L129" s="38" t="s">
-        <v>272</v>
-      </c>
+      <c r="L129" s="38"/>
       <c r="M129" s="38"/>
       <c r="N129" s="38"/>
       <c r="O129" s="38"/>
@@ -8780,22 +8763,22 @@
         <v>61</v>
       </c>
       <c r="D130" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="E130" s="43" t="s">
         <v>293</v>
-      </c>
-      <c r="E130" s="43" t="s">
-        <v>294</v>
       </c>
       <c r="F130" s="37">
         <v>46011</v>
       </c>
       <c r="G130" s="37" t="s">
+        <v>482</v>
+      </c>
+      <c r="H130" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="H130" s="37" t="s">
+      <c r="I130" s="42" t="s">
         <v>484</v>
-      </c>
-      <c r="I130" s="42" t="s">
-        <v>485</v>
       </c>
       <c r="J130" s="38" t="s">
         <v>64</v>
@@ -8809,7 +8792,7 @@
         <v>64</v>
       </c>
       <c r="O130" s="38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P130" s="38" t="s">
         <v>64</v>
@@ -8841,10 +8824,10 @@
         <v>57</v>
       </c>
       <c r="D131" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="E131" s="43" t="s">
         <v>295</v>
-      </c>
-      <c r="E131" s="43" t="s">
-        <v>296</v>
       </c>
       <c r="F131" s="37"/>
       <c r="G131" s="37"/>
@@ -8878,10 +8861,10 @@
         <v>57</v>
       </c>
       <c r="D132" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="E132" s="43" t="s">
         <v>297</v>
-      </c>
-      <c r="E132" s="43" t="s">
-        <v>298</v>
       </c>
       <c r="F132" s="37"/>
       <c r="G132" s="37"/>
@@ -8915,10 +8898,10 @@
         <v>57</v>
       </c>
       <c r="D133" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="E133" s="43" t="s">
         <v>299</v>
-      </c>
-      <c r="E133" s="43" t="s">
-        <v>300</v>
       </c>
       <c r="F133" s="37"/>
       <c r="G133" s="37"/>
@@ -8952,10 +8935,10 @@
         <v>57</v>
       </c>
       <c r="D134" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="E134" s="43" t="s">
         <v>301</v>
-      </c>
-      <c r="E134" s="43" t="s">
-        <v>302</v>
       </c>
       <c r="F134" s="37"/>
       <c r="G134" s="37"/>
@@ -8989,10 +8972,10 @@
         <v>57</v>
       </c>
       <c r="D135" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="E135" s="43" t="s">
         <v>303</v>
-      </c>
-      <c r="E135" s="43" t="s">
-        <v>304</v>
       </c>
       <c r="F135" s="37"/>
       <c r="G135" s="37"/>
@@ -9026,10 +9009,10 @@
         <v>57</v>
       </c>
       <c r="D136" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="E136" s="43" t="s">
         <v>305</v>
-      </c>
-      <c r="E136" s="43" t="s">
-        <v>306</v>
       </c>
       <c r="F136" s="37"/>
       <c r="G136" s="37"/>
@@ -9063,10 +9046,10 @@
         <v>57</v>
       </c>
       <c r="D137" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="E137" s="43" t="s">
         <v>307</v>
-      </c>
-      <c r="E137" s="43" t="s">
-        <v>308</v>
       </c>
       <c r="F137" s="37"/>
       <c r="G137" s="37"/>
@@ -9100,10 +9083,10 @@
         <v>57</v>
       </c>
       <c r="D138" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="E138" s="43" t="s">
         <v>309</v>
-      </c>
-      <c r="E138" s="43" t="s">
-        <v>310</v>
       </c>
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
@@ -9137,10 +9120,10 @@
         <v>57</v>
       </c>
       <c r="D139" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="E139" s="43" t="s">
         <v>311</v>
-      </c>
-      <c r="E139" s="43" t="s">
-        <v>312</v>
       </c>
       <c r="F139" s="37"/>
       <c r="G139" s="37"/>
@@ -9174,10 +9157,10 @@
         <v>57</v>
       </c>
       <c r="D140" s="35" t="s">
+        <v>312</v>
+      </c>
+      <c r="E140" s="43" t="s">
         <v>313</v>
-      </c>
-      <c r="E140" s="43" t="s">
-        <v>314</v>
       </c>
       <c r="F140" s="37"/>
       <c r="G140" s="37"/>
@@ -9211,10 +9194,10 @@
         <v>57</v>
       </c>
       <c r="D141" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="E141" s="43" t="s">
         <v>315</v>
-      </c>
-      <c r="E141" s="43" t="s">
-        <v>316</v>
       </c>
       <c r="F141" s="37"/>
       <c r="G141" s="37"/>
@@ -9248,10 +9231,10 @@
         <v>57</v>
       </c>
       <c r="D142" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="E142" s="43" t="s">
         <v>317</v>
-      </c>
-      <c r="E142" s="43" t="s">
-        <v>318</v>
       </c>
       <c r="F142" s="37"/>
       <c r="G142" s="37"/>
@@ -9285,10 +9268,10 @@
         <v>57</v>
       </c>
       <c r="D143" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="E143" s="43" t="s">
         <v>319</v>
-      </c>
-      <c r="E143" s="43" t="s">
-        <v>320</v>
       </c>
       <c r="F143" s="37"/>
       <c r="G143" s="37"/>
@@ -9322,10 +9305,10 @@
         <v>57</v>
       </c>
       <c r="D144" s="35" t="s">
+        <v>320</v>
+      </c>
+      <c r="E144" s="43" t="s">
         <v>321</v>
-      </c>
-      <c r="E144" s="43" t="s">
-        <v>322</v>
       </c>
       <c r="F144" s="37"/>
       <c r="G144" s="37"/>
@@ -9359,10 +9342,10 @@
         <v>57</v>
       </c>
       <c r="D145" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="E145" s="43" t="s">
         <v>323</v>
-      </c>
-      <c r="E145" s="43" t="s">
-        <v>324</v>
       </c>
       <c r="F145" s="37"/>
       <c r="G145" s="37"/>
@@ -9396,10 +9379,10 @@
         <v>48</v>
       </c>
       <c r="D146" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="E146" s="43" t="s">
         <v>325</v>
-      </c>
-      <c r="E146" s="43" t="s">
-        <v>326</v>
       </c>
       <c r="F146" s="37"/>
       <c r="G146" s="37"/>
@@ -9433,10 +9416,10 @@
         <v>48</v>
       </c>
       <c r="D147" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="E147" s="43" t="s">
         <v>327</v>
-      </c>
-      <c r="E147" s="43" t="s">
-        <v>328</v>
       </c>
       <c r="F147" s="37"/>
       <c r="G147" s="37"/>
@@ -9467,13 +9450,13 @@
         <v>47</v>
       </c>
       <c r="C148" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="D148" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="D148" s="35" t="s">
+      <c r="E148" s="43" t="s">
         <v>330</v>
-      </c>
-      <c r="E148" s="43" t="s">
-        <v>331</v>
       </c>
       <c r="F148" s="37"/>
       <c r="G148" s="37"/>
@@ -9504,13 +9487,13 @@
         <v>47</v>
       </c>
       <c r="C149" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D149" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="E149" s="43" t="s">
         <v>332</v>
-      </c>
-      <c r="E149" s="43" t="s">
-        <v>333</v>
       </c>
       <c r="F149" s="37"/>
       <c r="G149" s="37"/>
@@ -9541,13 +9524,13 @@
         <v>47</v>
       </c>
       <c r="C150" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D150" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="E150" s="43" t="s">
         <v>334</v>
-      </c>
-      <c r="E150" s="43" t="s">
-        <v>335</v>
       </c>
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
@@ -9578,10 +9561,10 @@
         <v>47</v>
       </c>
       <c r="C151" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D151" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E151" s="43" t="s">
         <v>53</v>
@@ -9615,10 +9598,10 @@
         <v>47</v>
       </c>
       <c r="C152" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D152" s="35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E152" s="43" t="s">
         <v>75</v>
@@ -9652,13 +9635,13 @@
         <v>47</v>
       </c>
       <c r="C153" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D153" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="E153" s="43" t="s">
         <v>338</v>
-      </c>
-      <c r="E153" s="43" t="s">
-        <v>339</v>
       </c>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
@@ -9689,13 +9672,13 @@
         <v>47</v>
       </c>
       <c r="C154" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D154" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="E154" s="43" t="s">
         <v>340</v>
-      </c>
-      <c r="E154" s="43" t="s">
-        <v>341</v>
       </c>
       <c r="F154" s="37"/>
       <c r="G154" s="37"/>
@@ -9726,13 +9709,13 @@
         <v>47</v>
       </c>
       <c r="C155" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D155" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="E155" s="43" t="s">
         <v>342</v>
-      </c>
-      <c r="E155" s="43" t="s">
-        <v>343</v>
       </c>
       <c r="F155" s="37"/>
       <c r="G155" s="37"/>
@@ -9763,13 +9746,13 @@
         <v>47</v>
       </c>
       <c r="C156" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D156" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="E156" s="43" t="s">
         <v>344</v>
-      </c>
-      <c r="E156" s="43" t="s">
-        <v>345</v>
       </c>
       <c r="F156" s="37"/>
       <c r="G156" s="37"/>
@@ -9800,13 +9783,13 @@
         <v>47</v>
       </c>
       <c r="C157" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D157" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="E157" s="43" t="s">
         <v>346</v>
-      </c>
-      <c r="E157" s="43" t="s">
-        <v>347</v>
       </c>
       <c r="F157" s="37"/>
       <c r="G157" s="37"/>
@@ -9837,13 +9820,13 @@
         <v>47</v>
       </c>
       <c r="C158" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D158" s="35" t="s">
+        <v>347</v>
+      </c>
+      <c r="E158" s="43" t="s">
         <v>348</v>
-      </c>
-      <c r="E158" s="43" t="s">
-        <v>349</v>
       </c>
       <c r="F158" s="37"/>
       <c r="G158" s="37"/>
@@ -9874,13 +9857,13 @@
         <v>47</v>
       </c>
       <c r="C159" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D159" s="35" t="s">
+        <v>349</v>
+      </c>
+      <c r="E159" s="43" t="s">
         <v>350</v>
-      </c>
-      <c r="E159" s="43" t="s">
-        <v>351</v>
       </c>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
@@ -9911,13 +9894,13 @@
         <v>47</v>
       </c>
       <c r="C160" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D160" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="E160" s="43" t="s">
         <v>352</v>
-      </c>
-      <c r="E160" s="43" t="s">
-        <v>353</v>
       </c>
       <c r="F160" s="37"/>
       <c r="G160" s="37"/>
@@ -9948,13 +9931,13 @@
         <v>47</v>
       </c>
       <c r="C161" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D161" s="35" t="s">
+        <v>353</v>
+      </c>
+      <c r="E161" s="43" t="s">
         <v>354</v>
-      </c>
-      <c r="E161" s="43" t="s">
-        <v>355</v>
       </c>
       <c r="F161" s="37"/>
       <c r="G161" s="37"/>
@@ -9985,13 +9968,13 @@
         <v>47</v>
       </c>
       <c r="C162" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D162" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="E162" s="43" t="s">
         <v>356</v>
-      </c>
-      <c r="E162" s="43" t="s">
-        <v>357</v>
       </c>
       <c r="F162" s="37"/>
       <c r="G162" s="37"/>
@@ -10022,13 +10005,13 @@
         <v>47</v>
       </c>
       <c r="C163" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D163" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="E163" s="43" t="s">
         <v>358</v>
-      </c>
-      <c r="E163" s="43" t="s">
-        <v>359</v>
       </c>
       <c r="F163" s="37"/>
       <c r="G163" s="37"/>
@@ -10062,22 +10045,22 @@
         <v>61</v>
       </c>
       <c r="D164" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="E164" s="43" t="s">
         <v>360</v>
-      </c>
-      <c r="E164" s="43" t="s">
-        <v>361</v>
       </c>
       <c r="F164" s="37">
         <v>46011</v>
       </c>
       <c r="G164" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="H164" s="37" t="s">
         <v>486</v>
       </c>
-      <c r="H164" s="37" t="s">
+      <c r="I164" s="42" t="s">
         <v>487</v>
-      </c>
-      <c r="I164" s="42" t="s">
-        <v>488</v>
       </c>
       <c r="J164" s="38" t="s">
         <v>64</v>
@@ -10109,22 +10092,22 @@
         <v>61</v>
       </c>
       <c r="D165" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="E165" s="43" t="s">
         <v>362</v>
-      </c>
-      <c r="E165" s="43" t="s">
-        <v>363</v>
       </c>
       <c r="F165" s="37">
         <v>46011</v>
       </c>
       <c r="G165" s="37" t="s">
+        <v>488</v>
+      </c>
+      <c r="H165" s="37" t="s">
         <v>489</v>
       </c>
-      <c r="H165" s="37" t="s">
+      <c r="I165" s="42" t="s">
         <v>490</v>
-      </c>
-      <c r="I165" s="42" t="s">
-        <v>491</v>
       </c>
       <c r="J165" s="38" t="s">
         <v>64</v>
@@ -10155,10 +10138,10 @@
         <v>55</v>
       </c>
       <c r="D166" s="35" t="s">
+        <v>363</v>
+      </c>
+      <c r="E166" s="43" t="s">
         <v>364</v>
-      </c>
-      <c r="E166" s="43" t="s">
-        <v>365</v>
       </c>
       <c r="F166" s="37"/>
       <c r="G166" s="37"/>
@@ -10192,10 +10175,10 @@
         <v>55</v>
       </c>
       <c r="D167" s="35" t="s">
+        <v>365</v>
+      </c>
+      <c r="E167" s="43" t="s">
         <v>366</v>
-      </c>
-      <c r="E167" s="43" t="s">
-        <v>367</v>
       </c>
       <c r="F167" s="37"/>
       <c r="G167" s="37"/>
@@ -10229,10 +10212,10 @@
         <v>48</v>
       </c>
       <c r="D168" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="E168" s="43" t="s">
         <v>368</v>
-      </c>
-      <c r="E168" s="43" t="s">
-        <v>369</v>
       </c>
       <c r="F168" s="37"/>
       <c r="G168" s="37"/>
@@ -10266,10 +10249,10 @@
         <v>72</v>
       </c>
       <c r="D169" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="E169" s="43" t="s">
         <v>370</v>
-      </c>
-      <c r="E169" s="43" t="s">
-        <v>371</v>
       </c>
       <c r="F169" s="37"/>
       <c r="G169" s="37"/>
@@ -10303,10 +10286,10 @@
         <v>72</v>
       </c>
       <c r="D170" s="35" t="s">
+        <v>371</v>
+      </c>
+      <c r="E170" s="43" t="s">
         <v>372</v>
-      </c>
-      <c r="E170" s="43" t="s">
-        <v>373</v>
       </c>
       <c r="F170" s="37"/>
       <c r="G170" s="37"/>
@@ -10340,10 +10323,10 @@
         <v>70</v>
       </c>
       <c r="D171" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="E171" s="43" t="s">
         <v>374</v>
-      </c>
-      <c r="E171" s="43" t="s">
-        <v>375</v>
       </c>
       <c r="F171" s="37"/>
       <c r="G171" s="37"/>
@@ -10377,10 +10360,10 @@
         <v>70</v>
       </c>
       <c r="D172" s="35" t="s">
+        <v>375</v>
+      </c>
+      <c r="E172" s="43" t="s">
         <v>376</v>
-      </c>
-      <c r="E172" s="43" t="s">
-        <v>377</v>
       </c>
       <c r="F172" s="37"/>
       <c r="G172" s="37"/>
@@ -10414,10 +10397,10 @@
         <v>68</v>
       </c>
       <c r="D173" s="35" t="s">
+        <v>377</v>
+      </c>
+      <c r="E173" s="43" t="s">
         <v>378</v>
-      </c>
-      <c r="E173" s="43" t="s">
-        <v>379</v>
       </c>
       <c r="F173" s="37"/>
       <c r="G173" s="37"/>
@@ -10451,10 +10434,10 @@
         <v>68</v>
       </c>
       <c r="D174" s="35" t="s">
+        <v>379</v>
+      </c>
+      <c r="E174" s="43" t="s">
         <v>380</v>
-      </c>
-      <c r="E174" s="43" t="s">
-        <v>381</v>
       </c>
       <c r="F174" s="37"/>
       <c r="G174" s="37"/>
@@ -10485,13 +10468,13 @@
         <v>47</v>
       </c>
       <c r="C175" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D175" s="35" t="s">
+        <v>381</v>
+      </c>
+      <c r="E175" s="43" t="s">
         <v>382</v>
-      </c>
-      <c r="E175" s="43" t="s">
-        <v>383</v>
       </c>
       <c r="F175" s="37"/>
       <c r="G175" s="37"/>
@@ -10525,10 +10508,10 @@
         <v>61</v>
       </c>
       <c r="D176" s="35" t="s">
+        <v>383</v>
+      </c>
+      <c r="E176" s="43" t="s">
         <v>384</v>
-      </c>
-      <c r="E176" s="43" t="s">
-        <v>385</v>
       </c>
       <c r="F176" s="37"/>
       <c r="G176" s="37"/>
@@ -10538,7 +10521,7 @@
         <v>66</v>
       </c>
       <c r="K176" s="38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L176" s="35"/>
       <c r="M176" s="38"/>
@@ -10548,10 +10531,10 @@
       <c r="Q176" s="38"/>
       <c r="R176" s="38"/>
       <c r="S176" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="T176" s="38" t="s">
         <v>387</v>
-      </c>
-      <c r="T176" s="38" t="s">
-        <v>388</v>
       </c>
       <c r="U176" s="35"/>
       <c r="V176" s="35"/>
@@ -10570,10 +10553,10 @@
         <v>59</v>
       </c>
       <c r="D177" s="35" t="s">
+        <v>388</v>
+      </c>
+      <c r="E177" s="43" t="s">
         <v>389</v>
-      </c>
-      <c r="E177" s="43" t="s">
-        <v>390</v>
       </c>
       <c r="F177" s="35"/>
       <c r="G177" s="35"/>
@@ -10607,10 +10590,10 @@
         <v>72</v>
       </c>
       <c r="D178" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="E178" s="43" t="s">
         <v>391</v>
-      </c>
-      <c r="E178" s="43" t="s">
-        <v>392</v>
       </c>
       <c r="F178" s="35"/>
       <c r="G178" s="35"/>
@@ -10644,10 +10627,10 @@
         <v>68</v>
       </c>
       <c r="D179" s="35" t="s">
+        <v>392</v>
+      </c>
+      <c r="E179" s="43" t="s">
         <v>393</v>
-      </c>
-      <c r="E179" s="43" t="s">
-        <v>394</v>
       </c>
       <c r="F179" s="35"/>
       <c r="G179" s="35"/>
@@ -10681,10 +10664,10 @@
         <v>70</v>
       </c>
       <c r="D180" s="35" t="s">
+        <v>394</v>
+      </c>
+      <c r="E180" s="43" t="s">
         <v>395</v>
-      </c>
-      <c r="E180" s="43" t="s">
-        <v>396</v>
       </c>
       <c r="F180" s="35"/>
       <c r="G180" s="35"/>
@@ -10718,10 +10701,10 @@
         <v>48</v>
       </c>
       <c r="D181" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="E181" s="44" t="s">
         <v>397</v>
-      </c>
-      <c r="E181" s="44" t="s">
-        <v>398</v>
       </c>
       <c r="F181" s="35"/>
       <c r="G181" s="35"/>
@@ -10755,10 +10738,10 @@
         <v>55</v>
       </c>
       <c r="D182" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="E182" s="43" t="s">
         <v>399</v>
-      </c>
-      <c r="E182" s="43" t="s">
-        <v>400</v>
       </c>
       <c r="F182" s="35"/>
       <c r="G182" s="35"/>
@@ -10792,10 +10775,10 @@
         <v>61</v>
       </c>
       <c r="D183" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="E183" s="43" t="s">
         <v>401</v>
-      </c>
-      <c r="E183" s="43" t="s">
-        <v>402</v>
       </c>
       <c r="F183" s="37"/>
       <c r="G183" s="37"/>
@@ -10805,7 +10788,7 @@
         <v>66</v>
       </c>
       <c r="K183" s="38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L183" s="35"/>
       <c r="M183" s="38"/>
@@ -10815,10 +10798,10 @@
       <c r="Q183" s="38"/>
       <c r="R183" s="38"/>
       <c r="S183" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="T183" s="38" t="s">
         <v>387</v>
-      </c>
-      <c r="T183" s="38" t="s">
-        <v>388</v>
       </c>
       <c r="U183" s="35"/>
       <c r="V183" s="35"/>
@@ -10837,10 +10820,10 @@
         <v>57</v>
       </c>
       <c r="D184" s="35" t="s">
+        <v>402</v>
+      </c>
+      <c r="E184" s="43" t="s">
         <v>403</v>
-      </c>
-      <c r="E184" s="43" t="s">
-        <v>404</v>
       </c>
       <c r="F184" s="35"/>
       <c r="G184" s="35"/>
@@ -10871,13 +10854,13 @@
         <v>47</v>
       </c>
       <c r="C185" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D185" s="35" t="s">
+        <v>404</v>
+      </c>
+      <c r="E185" s="43" t="s">
         <v>405</v>
-      </c>
-      <c r="E185" s="43" t="s">
-        <v>406</v>
       </c>
       <c r="F185" s="35"/>
       <c r="G185" s="35"/>
@@ -10911,10 +10894,10 @@
         <v>59</v>
       </c>
       <c r="D186" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="E186" s="43" t="s">
         <v>407</v>
-      </c>
-      <c r="E186" s="43" t="s">
-        <v>408</v>
       </c>
       <c r="F186" s="37"/>
       <c r="G186" s="37"/>
@@ -10948,10 +10931,10 @@
         <v>59</v>
       </c>
       <c r="D187" s="35" t="s">
+        <v>408</v>
+      </c>
+      <c r="E187" s="43" t="s">
         <v>409</v>
-      </c>
-      <c r="E187" s="43" t="s">
-        <v>410</v>
       </c>
       <c r="F187" s="37"/>
       <c r="G187" s="37"/>
@@ -10985,10 +10968,10 @@
         <v>48</v>
       </c>
       <c r="D188" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="E188" s="43" t="s">
         <v>411</v>
-      </c>
-      <c r="E188" s="43" t="s">
-        <v>412</v>
       </c>
       <c r="F188" s="37"/>
       <c r="G188" s="37"/>
@@ -11022,10 +11005,10 @@
         <v>59</v>
       </c>
       <c r="D189" s="35" t="s">
+        <v>412</v>
+      </c>
+      <c r="E189" s="43" t="s">
         <v>413</v>
-      </c>
-      <c r="E189" s="43" t="s">
-        <v>414</v>
       </c>
       <c r="F189" s="37"/>
       <c r="G189" s="37"/>
@@ -11059,10 +11042,10 @@
         <v>61</v>
       </c>
       <c r="D190" s="35" t="s">
+        <v>414</v>
+      </c>
+      <c r="E190" s="43" t="s">
         <v>415</v>
-      </c>
-      <c r="E190" s="43" t="s">
-        <v>416</v>
       </c>
       <c r="F190" s="37"/>
       <c r="G190" s="37"/>
@@ -11072,7 +11055,7 @@
         <v>66</v>
       </c>
       <c r="K190" s="38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L190" s="38"/>
       <c r="M190" s="38"/>
@@ -11082,10 +11065,10 @@
       <c r="Q190" s="38"/>
       <c r="R190" s="38"/>
       <c r="S190" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="T190" s="38" t="s">
         <v>387</v>
-      </c>
-      <c r="T190" s="38" t="s">
-        <v>388</v>
       </c>
       <c r="U190" s="39"/>
       <c r="V190" s="40"/>
@@ -11104,10 +11087,10 @@
         <v>57</v>
       </c>
       <c r="D191" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="E191" s="43" t="s">
         <v>417</v>
-      </c>
-      <c r="E191" s="43" t="s">
-        <v>418</v>
       </c>
       <c r="F191" s="37"/>
       <c r="G191" s="37"/>
@@ -11141,10 +11124,10 @@
         <v>57</v>
       </c>
       <c r="D192" s="35" t="s">
+        <v>418</v>
+      </c>
+      <c r="E192" s="43" t="s">
         <v>419</v>
-      </c>
-      <c r="E192" s="43" t="s">
-        <v>420</v>
       </c>
       <c r="F192" s="37"/>
       <c r="G192" s="37"/>
@@ -11178,10 +11161,10 @@
         <v>57</v>
       </c>
       <c r="D193" s="35" t="s">
+        <v>420</v>
+      </c>
+      <c r="E193" s="45" t="s">
         <v>421</v>
-      </c>
-      <c r="E193" s="45" t="s">
-        <v>422</v>
       </c>
       <c r="F193" s="37"/>
       <c r="G193" s="37"/>
@@ -15190,7 +15173,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -15200,32 +15183,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -15255,22 +15238,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>432</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15278,13 +15261,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="30" t="s">
         <v>435</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15292,13 +15275,13 @@
         <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>437</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15306,13 +15289,13 @@
         <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>439</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15320,13 +15303,13 @@
         <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>441</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15334,13 +15317,13 @@
         <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>443</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -15348,13 +15331,13 @@
         <v>72</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>445</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -15362,13 +15345,13 @@
         <v>61</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>447</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -15376,41 +15359,41 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>449</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="30" t="s">
         <v>452</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="D11" s="31" t="s">
         <v>454</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -16396,7 +16379,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>64</v>
@@ -16404,7 +16387,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>66</v>

</xml_diff>